<commit_message>
edits in student import
</commit_message>
<xml_diff>
--- a/downloads/excel-templates/users_template.xlsx
+++ b/downloads/excel-templates/users_template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -104,6 +104,15 @@
   </si>
   <si>
     <t>category_id</t>
+  </si>
+  <si>
+    <t>id_number</t>
+  </si>
+  <si>
+    <t>parent_name</t>
+  </si>
+  <si>
+    <t>salamaa</t>
   </si>
 </sst>
 </file>
@@ -449,18 +458,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="20" width="15.7109375" customWidth="1"/>
+    <col min="3" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" customWidth="1"/>
+    <col min="21" max="21" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,8 +529,14 @@
       <c r="S1" t="s">
         <v>16</v>
       </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -576,6 +593,12 @@
       </c>
       <c r="S2">
         <v>2</v>
+      </c>
+      <c r="T2">
+        <v>5556644422</v>
+      </c>
+      <c r="U2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added student id nu
</commit_message>
<xml_diff>
--- a/downloads/excel-templates/users_template.xlsx
+++ b/downloads/excel-templates/users_template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -106,13 +106,16 @@
     <t>category_id</t>
   </si>
   <si>
-    <t>id_number</t>
-  </si>
-  <si>
     <t>parent_name</t>
   </si>
   <si>
     <t>salamaa</t>
+  </si>
+  <si>
+    <t>parent_id_number</t>
+  </si>
+  <si>
+    <t>student_id_number</t>
   </si>
 </sst>
 </file>
@@ -458,20 +461,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="19" width="15.7109375" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" customWidth="1"/>
-    <col min="21" max="21" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="20" width="15.7109375" customWidth="1"/>
+    <col min="21" max="21" width="17.28515625" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,131 +483,137 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" t="s">
         <v>26</v>
       </c>
-      <c r="U1" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>1239874444</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1234567891</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>2</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>3</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>59</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>60</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>20</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>31028</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>36506</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>22</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>1</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>2</v>
       </c>
-      <c r="T2">
-        <v>5556644422</v>
-      </c>
-      <c r="U2" t="s">
-        <v>28</v>
+      <c r="U2">
+        <v>5356644422</v>
+      </c>
+      <c r="V2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
edit in students import and second edit in it && edit in teacher profile
</commit_message>
<xml_diff>
--- a/downloads/excel-templates/users_template.xlsx
+++ b/downloads/excel-templates/users_template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -79,27 +79,12 @@
     <t>current_semister</t>
   </si>
   <si>
-    <t>enjoyraj</t>
-  </si>
-  <si>
-    <t>enjoyraj@enjoyraj.com</t>
-  </si>
-  <si>
     <t>Test Address</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>Raj</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
-    <t>Enjoyssssssss</t>
-  </si>
-  <si>
     <t>branch_id</t>
   </si>
   <si>
@@ -109,13 +94,46 @@
     <t>parent_name</t>
   </si>
   <si>
-    <t>salamaa</t>
-  </si>
-  <si>
     <t>parent_id_number</t>
   </si>
   <si>
     <t>student_id_number</t>
+  </si>
+  <si>
+    <t>nationality</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>secondary_parent_id</t>
+  </si>
+  <si>
+    <t>secondary_parent_name</t>
+  </si>
+  <si>
+    <t>khaled hussain</t>
+  </si>
+  <si>
+    <t>new one</t>
+  </si>
+  <si>
+    <t>شهاب</t>
+  </si>
+  <si>
+    <t>new_1</t>
+  </si>
+  <si>
+    <t>ice_magic@gogo.com</t>
+  </si>
+  <si>
+    <t>shehab</t>
+  </si>
+  <si>
+    <t>ahmed</t>
+  </si>
+  <si>
+    <t>awd</t>
   </si>
 </sst>
 </file>
@@ -125,10 +143,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -151,14 +177,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -461,21 +490,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="20" width="15.7109375" customWidth="1"/>
-    <col min="21" max="21" width="17.28515625" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" customWidth="1"/>
+    <col min="4" max="21" width="15.7109375" customWidth="1"/>
+    <col min="22" max="22" width="17.28515625" customWidth="1"/>
+    <col min="23" max="23" width="12.5703125" customWidth="1"/>
+    <col min="24" max="24" width="20" customWidth="1"/>
+    <col min="25" max="25" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +514,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -498,13 +529,13 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
@@ -531,30 +562,39 @@
         <v>14</v>
       </c>
       <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" t="s">
-        <v>28</v>
-      </c>
       <c r="V1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" t="s">
         <v>26</v>
       </c>
+      <c r="Y1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C2">
-        <v>1239874444</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
+        <v>5555512345</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -563,7 +603,7 @@
         <v>1234567891</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -581,13 +621,13 @@
         <v>60</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="N2" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="O2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="P2" s="1">
         <v>31028</v>
@@ -596,19 +636,28 @@
         <v>36506</v>
       </c>
       <c r="R2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2">
+        <v>18</v>
+      </c>
+      <c r="S2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2">
         <v>1</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>2</v>
       </c>
-      <c r="U2">
-        <v>5356644422</v>
-      </c>
-      <c r="V2" t="s">
-        <v>27</v>
+      <c r="V2">
+        <v>6644885522</v>
+      </c>
+      <c r="W2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X2">
+        <v>5356644425</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>